<commit_message>
[#1199980645336559] code review changes
</commit_message>
<xml_diff>
--- a/pentaho/test/SP-0.2/test-case-17/inputs/input.xlsx
+++ b/pentaho/test/SP-0.2/test-case-17/inputs/input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon.ecung\Projects\data-warehouse\pentaho\test\SP-0.2\test-case-D\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon.ecung\Projects\data-warehouse\pentaho\test\SP-0.2\test-case-17\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6A6F42-558B-4E8E-A1ED-91DA2CE6613C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016563D5-F65D-4B0A-B57C-6E7DBCCCE559}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5955" yWindow="7515" windowWidth="13800" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -894,7 +894,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +935,7 @@
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>30825</v>
       </c>
       <c r="G2" t="s">

</xml_diff>